<commit_message>
Edited branch voice line
</commit_message>
<xml_diff>
--- a/Writing/Good Boy Voice Lines.xlsx
+++ b/Writing/Good Boy Voice Lines.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamie\Documents\Game Dev 1\Project 4\GameDevP4\Writing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laksj\Documents\Game Dev 1\Project 4\GameDevP4\Writing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548F7227-2E15-4E9B-AFCE-92500ECC3BF6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -298,9 +297,6 @@
     <t>Fetch - Part 3</t>
   </si>
   <si>
-    <t>That's *cough* that's a real nice branch, bud. Good job.</t>
-  </si>
-  <si>
     <t>Medication Time - Part 3</t>
   </si>
   <si>
@@ -380,12 +376,15 @@
   </si>
   <si>
     <t>Best day of my life. Paul tried for twenty minutes to get you into that picture, but you just kept running away. Remember?</t>
+  </si>
+  <si>
+    <t>That's *cough* that's real nice, bud. Good job.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -753,24 +752,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.28515625" customWidth="1"/>
-    <col min="3" max="3" width="57.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" customWidth="1"/>
+    <col min="3" max="3" width="57.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -790,7 +789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -804,7 +803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -818,7 +817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -832,7 +831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -846,7 +845,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -860,7 +859,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -874,7 +873,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -888,7 +887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
@@ -902,7 +901,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
@@ -916,7 +915,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
@@ -930,7 +929,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
@@ -941,7 +940,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
@@ -952,7 +951,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
@@ -963,7 +962,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
@@ -974,7 +973,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>18</v>
       </c>
@@ -985,7 +984,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>18</v>
       </c>
@@ -996,7 +995,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>18</v>
       </c>
@@ -1007,7 +1006,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>18</v>
       </c>
@@ -1018,7 +1017,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>18</v>
       </c>
@@ -1029,7 +1028,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>35</v>
       </c>
@@ -1040,7 +1039,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>35</v>
       </c>
@@ -1051,7 +1050,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>35</v>
       </c>
@@ -1062,7 +1061,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
@@ -1073,7 +1072,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>35</v>
       </c>
@@ -1084,7 +1083,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>35</v>
       </c>
@@ -1095,7 +1094,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>35</v>
       </c>
@@ -1106,7 +1105,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>35</v>
       </c>
@@ -1117,7 +1116,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>35</v>
       </c>
@@ -1128,7 +1127,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>18</v>
       </c>
@@ -1139,7 +1138,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>18</v>
       </c>
@@ -1150,7 +1149,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>18</v>
       </c>
@@ -1161,7 +1160,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>18</v>
       </c>
@@ -1172,7 +1171,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>18</v>
       </c>
@@ -1183,7 +1182,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>53</v>
       </c>
@@ -1194,7 +1193,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>55</v>
       </c>
@@ -1205,7 +1204,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>55</v>
       </c>
@@ -1216,7 +1215,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>55</v>
       </c>
@@ -1227,7 +1226,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>60</v>
       </c>
@@ -1238,7 +1237,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>60</v>
       </c>
@@ -1249,7 +1248,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>65</v>
       </c>
@@ -1260,7 +1259,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>65</v>
       </c>
@@ -1271,7 +1270,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>65</v>
       </c>
@@ -1282,7 +1281,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>65</v>
       </c>
@@ -1293,7 +1292,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>65</v>
       </c>
@@ -1304,7 +1303,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>65</v>
       </c>
@@ -1315,7 +1314,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>65</v>
       </c>
@@ -1326,7 +1325,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>65</v>
       </c>
@@ -1337,7 +1336,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>65</v>
       </c>
@@ -1348,7 +1347,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>65</v>
       </c>
@@ -1359,7 +1358,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>65</v>
       </c>
@@ -1370,7 +1369,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>65</v>
       </c>
@@ -1381,7 +1380,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>65</v>
       </c>
@@ -1392,7 +1391,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>65</v>
       </c>
@@ -1403,7 +1402,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>65</v>
       </c>
@@ -1414,7 +1413,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>65</v>
       </c>
@@ -1425,7 +1424,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>90</v>
       </c>
@@ -1433,161 +1432,161 @@
         <v>91</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>90</v>
       </c>
       <c r="B63" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C63" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>90</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>90</v>
       </c>
       <c r="B65" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C65" s="4" t="s">
+    </row>
+    <row r="66" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="C66" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C66" s="4" t="s">
+    </row>
+    <row r="67" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B67" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B67" s="4" t="s">
+      <c r="C67" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C67" s="4" t="s">
+    </row>
+    <row r="68" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B68" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B68" s="4" t="s">
+      <c r="C68" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C69" s="4" t="s">
+    </row>
+    <row r="70" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B70" s="4" t="s">
+      <c r="C70" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C70" s="4" t="s">
+    </row>
+    <row r="71" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B71" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B71" s="4" t="s">
+      <c r="C71" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C71" s="4" t="s">
+    </row>
+    <row r="72" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B72" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A72" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B72" s="4" t="s">
+      <c r="C72" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C72" s="4" t="s">
+    </row>
+    <row r="73" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B75" s="4" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B75" s="4" t="s">
+      <c r="C75" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C75" s="4" t="s">
+    </row>
+    <row r="76" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B76" s="4" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B76" s="4" t="s">
+      <c r="C76" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started Photos Folder, edited voice lines, tagged cuts in narrative doc.
</commit_message>
<xml_diff>
--- a/Writing/Good Boy Voice Lines.xlsx
+++ b/Writing/Good Boy Voice Lines.xlsx
@@ -348,9 +348,6 @@
     <t>Inspect Photo - 70s NY Thing</t>
   </si>
   <si>
-    <t>I almost forgot about that one. I think that's right around when Paul and I met.</t>
-  </si>
-  <si>
     <t>Inspect Item - Hiking Backpack</t>
   </si>
   <si>
@@ -379,6 +376,9 @@
   </si>
   <si>
     <t>That's *cough* that's real nice, bud. Good job.</t>
+  </si>
+  <si>
+    <t>My trip to Central Park! That's right around when Paul and I met. I just couldn't believe how many people there were.</t>
   </si>
 </sst>
 </file>
@@ -758,8 +758,8 @@
   </sheetPr>
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1432,7 +1432,7 @@
         <v>91</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -1498,7 +1498,7 @@
         <v>102</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -1542,7 +1542,7 @@
         <v>108</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -1550,10 +1550,10 @@
         <v>97</v>
       </c>
       <c r="B73" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -1561,10 +1561,10 @@
         <v>97</v>
       </c>
       <c r="B74" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C74" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -1572,10 +1572,10 @@
         <v>97</v>
       </c>
       <c r="B75" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C75" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -1583,10 +1583,10 @@
         <v>97</v>
       </c>
       <c r="B76" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C76" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trimmed and condensed photos. Cut and revised voice lines to match.
</commit_message>
<xml_diff>
--- a/Writing/Good Boy Voice Lines.xlsx
+++ b/Writing/Good Boy Voice Lines.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laksj\Documents\Game Dev 1\Project 4\GameDevP4\Writing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamie\Documents\Game Dev 1\Project 4\GameDevP4\Writing\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9208BA3-236B-4EBE-9F00-C3896564C860}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="137">
   <si>
     <t>Part</t>
   </si>
@@ -315,9 +316,6 @@
     <t>All Parts</t>
   </si>
   <si>
-    <t>Inspect Photo - Owner and Partner</t>
-  </si>
-  <si>
     <t>I know, bud. I miss him, too.</t>
   </si>
   <si>
@@ -379,13 +377,67 @@
   </si>
   <si>
     <t>My trip to Central Park! That's right around when Paul and I met. I just couldn't believe how many people there were.</t>
+  </si>
+  <si>
+    <t>Replaced</t>
+  </si>
+  <si>
+    <t>Inspect Photo - Halloween Party</t>
+  </si>
+  <si>
+    <t>Paul's first Halloween with us. He and the guys really hit it off.</t>
+  </si>
+  <si>
+    <t>That was supposed to be a family photo, remember? Paul just couldn't get you to stay in frame!</t>
+  </si>
+  <si>
+    <t>Inspect Photo - Paul with Baby</t>
+  </si>
+  <si>
+    <t>Paul always wanted kids. I guess you and his nephew were the closest he could get.</t>
+  </si>
+  <si>
+    <t>Inspect Photo - Crazy Paul</t>
+  </si>
+  <si>
+    <t>Inspect Photo - Drinks</t>
+  </si>
+  <si>
+    <t>He really was one hell of a crazy guy. I don't think he could sit for more than one photo without making some kinda face.</t>
+  </si>
+  <si>
+    <t>I think that's the last time we went out together. It just got too hard after that.</t>
+  </si>
+  <si>
+    <t>Inspect Photo - Camping (Duo)</t>
+  </si>
+  <si>
+    <t>Inspect Photo - Oscar Truck</t>
+  </si>
+  <si>
+    <t>Damn, my hair really did look better back then.</t>
+  </si>
+  <si>
+    <t>Inspect Photo - Camping (Group)</t>
+  </si>
+  <si>
+    <t>Not pictured - Paul running off to keep your ass from jumping in the river.</t>
+  </si>
+  <si>
+    <t>Inspect Photo - Wedding</t>
+  </si>
+  <si>
+    <t>Inspect Photo - Lobster Paul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Betty and Jim's wedding. See us there, upper left? You know, they kept asking us when we were gonna tie it. I should give 'em a call. It's been too long. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -400,8 +452,13 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -420,6 +477,18 @@
         <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -433,12 +502,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -752,24 +826,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="34.33203125" customWidth="1"/>
-    <col min="3" max="3" width="57.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
+    <col min="3" max="3" width="57.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -788,8 +862,11 @@
       <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -803,7 +880,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -817,7 +894,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -831,7 +908,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -845,7 +922,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -859,7 +936,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -873,7 +950,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -887,7 +964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
@@ -901,7 +978,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
@@ -915,7 +992,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
@@ -929,7 +1006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
@@ -940,7 +1017,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
@@ -951,7 +1028,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
@@ -962,7 +1039,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
@@ -973,7 +1050,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>18</v>
       </c>
@@ -984,7 +1061,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>18</v>
       </c>
@@ -995,7 +1072,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>18</v>
       </c>
@@ -1006,7 +1083,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>18</v>
       </c>
@@ -1017,7 +1094,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>18</v>
       </c>
@@ -1028,7 +1105,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>35</v>
       </c>
@@ -1039,7 +1116,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>35</v>
       </c>
@@ -1050,7 +1127,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>35</v>
       </c>
@@ -1061,7 +1138,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
@@ -1072,7 +1149,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>35</v>
       </c>
@@ -1083,7 +1160,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>35</v>
       </c>
@@ -1094,7 +1171,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>35</v>
       </c>
@@ -1105,7 +1182,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>35</v>
       </c>
@@ -1116,7 +1193,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>35</v>
       </c>
@@ -1127,7 +1204,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>18</v>
       </c>
@@ -1138,7 +1215,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>18</v>
       </c>
@@ -1149,7 +1226,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>18</v>
       </c>
@@ -1160,7 +1237,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>18</v>
       </c>
@@ -1171,7 +1248,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>18</v>
       </c>
@@ -1182,7 +1259,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>53</v>
       </c>
@@ -1193,7 +1270,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>55</v>
       </c>
@@ -1204,7 +1281,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>55</v>
       </c>
@@ -1215,7 +1292,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>55</v>
       </c>
@@ -1226,7 +1303,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>60</v>
       </c>
@@ -1237,7 +1314,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>60</v>
       </c>
@@ -1248,7 +1325,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>65</v>
       </c>
@@ -1259,7 +1336,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>65</v>
       </c>
@@ -1270,7 +1347,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>65</v>
       </c>
@@ -1281,7 +1358,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>65</v>
       </c>
@@ -1292,7 +1369,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>65</v>
       </c>
@@ -1303,7 +1380,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>65</v>
       </c>
@@ -1314,7 +1391,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>65</v>
       </c>
@@ -1325,7 +1402,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>65</v>
       </c>
@@ -1336,7 +1413,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>65</v>
       </c>
@@ -1347,7 +1424,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>65</v>
       </c>
@@ -1358,7 +1435,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>65</v>
       </c>
@@ -1369,7 +1446,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>65</v>
       </c>
@@ -1380,7 +1457,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>65</v>
       </c>
@@ -1391,7 +1468,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>65</v>
       </c>
@@ -1402,7 +1479,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>65</v>
       </c>
@@ -1413,7 +1490,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>65</v>
       </c>
@@ -1424,7 +1501,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>90</v>
       </c>
@@ -1432,10 +1509,10 @@
         <v>91</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>90</v>
       </c>
@@ -1446,7 +1523,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>90</v>
       </c>
@@ -1457,7 +1534,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>90</v>
       </c>
@@ -1468,128 +1545,227 @@
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C66" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C66" s="4" t="s">
+    </row>
+    <row r="67" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B67" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B67" s="4" t="s">
+      <c r="C67" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C67" s="4" t="s">
+    </row>
+    <row r="68" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A68" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B68" s="6" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B68" s="4" t="s">
+      <c r="C68" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A69" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C69" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C69" s="4" t="s">
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A70" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B70" s="6" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B70" s="4" t="s">
+      <c r="C70" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="D70" s="5"/>
+    </row>
+    <row r="71" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A71" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B71" s="7" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B71" s="4" t="s">
+      <c r="C71" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+    </row>
+    <row r="72" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B72" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B72" s="4" t="s">
+      <c r="C72" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B75" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C72" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B75" s="4" t="s">
+      <c r="C75" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C75" s="4" t="s">
+    </row>
+    <row r="76" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B76" s="4" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B76" s="4" t="s">
+      <c r="C76" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C76" s="4" t="s">
-        <v>112</v>
+    </row>
+    <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>